<commit_message>
Completed data exploration (Q1–Q5) and added initial observations
</commit_message>
<xml_diff>
--- a/data/foodhub_order.xlsx
+++ b/data/foodhub_order.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/bf891bf09a799b20/Data Analytics/Python/FoodHub/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/bf891bf09a799b20/DataAnalytics/Python/FoodHub/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="0" documentId="8_{64E6E1D9-BDB5-47F1-9F78-93007192BD7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{5BAA1057-82F7-459F-B01D-6D1C5E63EE43}"/>
+    <workbookView xWindow="-23136" yWindow="3216" windowWidth="23232" windowHeight="13872" xr2:uid="{5BAA1057-82F7-459F-B01D-6D1C5E63EE43}"/>
   </bookViews>
   <sheets>
     <sheet name="foodhub_order" sheetId="1" r:id="rId1"/>
@@ -1505,7 +1505,7 @@
   <dimension ref="A1:I1899"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Completed questions 6–11: univariate analysis and insights
</commit_message>
<xml_diff>
--- a/data/foodhub_order.xlsx
+++ b/data/foodhub_order.xlsx
@@ -8,22 +8,36 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/bf891bf09a799b20/DataAnalytics/Python/FoodHub/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{64E6E1D9-BDB5-47F1-9F78-93007192BD7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="45" documentId="8_{64E6E1D9-BDB5-47F1-9F78-93007192BD7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1185E050-C3C4-4CAD-A18E-5BC98C2A3189}"/>
   <bookViews>
     <workbookView xWindow="-23136" yWindow="3216" windowWidth="23232" windowHeight="13872" xr2:uid="{5BAA1057-82F7-459F-B01D-6D1C5E63EE43}"/>
   </bookViews>
   <sheets>
     <sheet name="foodhub_order" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">foodhub_order!$A$1:$I$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">foodhub_order!$A$1:$I$1899</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6439" uniqueCount="204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6499" uniqueCount="215">
   <si>
     <t>order_id</t>
   </si>
@@ -636,12 +650,45 @@
   <si>
     <t>'wichcraft</t>
   </si>
+  <si>
+    <t>count</t>
+  </si>
+  <si>
+    <t>unique</t>
+  </si>
+  <si>
+    <t>top</t>
+  </si>
+  <si>
+    <t>freq</t>
+  </si>
+  <si>
+    <t>mean</t>
+  </si>
+  <si>
+    <t>std</t>
+  </si>
+  <si>
+    <t>min</t>
+  </si>
+  <si>
+    <t>max</t>
+  </si>
+  <si>
+    <t>NaN</t>
+  </si>
+  <si>
+    <t>&lt;NA&gt;</t>
+  </si>
+  <si>
+    <t>Mode</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -776,8 +823,26 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="34">
+  <fills count="36">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -963,8 +1028,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -1079,6 +1156,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1124,9 +1216,26 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="13" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="20" fillId="33" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="34" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="35" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1505,7 +1614,7 @@
   <dimension ref="A1:I1899"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -56592,7 +56701,450 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:I1" xr:uid="{51B2ACA2-0467-45E3-B735-4A297B099BB0}"/>
+  <autoFilter ref="A1:I1899" xr:uid="{51B2ACA2-0467-45E3-B735-4A297B099BB0}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12FE62BD-8D0C-4C9B-84A7-4E0BFB35BDE9}">
+  <dimension ref="A1:M12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K13" sqref="K13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="29.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="23.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.28515625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="12.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="12.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9" style="2" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="5.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="14" max="16384" width="29.5703125" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A1" s="1"/>
+      <c r="B1" s="4" t="s">
+        <v>204</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>205</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>206</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>210</v>
+      </c>
+      <c r="I1" s="5">
+        <v>0.25</v>
+      </c>
+      <c r="J1" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="K1" s="5">
+        <v>0.75</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>211</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="3">
+        <v>1898</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="F2" s="3">
+        <v>1477495.5</v>
+      </c>
+      <c r="G2" s="3">
+        <v>548.04972399999997</v>
+      </c>
+      <c r="H2" s="3">
+        <v>1476547</v>
+      </c>
+      <c r="I2" s="3">
+        <v>1477021.25</v>
+      </c>
+      <c r="J2" s="3">
+        <v>1477495.5</v>
+      </c>
+      <c r="K2" s="3">
+        <v>1477969.75</v>
+      </c>
+      <c r="L2" s="3">
+        <v>1478444</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="3">
+        <v>1898</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="F3" s="3">
+        <v>171168.47839800001</v>
+      </c>
+      <c r="G3" s="3">
+        <v>113698.13974300001</v>
+      </c>
+      <c r="H3" s="3">
+        <v>1311</v>
+      </c>
+      <c r="I3" s="3">
+        <v>77787.75</v>
+      </c>
+      <c r="J3" s="3">
+        <v>128600</v>
+      </c>
+      <c r="K3" s="3">
+        <v>270525</v>
+      </c>
+      <c r="L3" s="3">
+        <v>405334</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="3">
+        <v>1898</v>
+      </c>
+      <c r="C4" s="3">
+        <v>178</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="E4" s="3">
+        <v>219</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="K4" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="L4" s="3" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="3">
+        <v>1898</v>
+      </c>
+      <c r="C5" s="3">
+        <v>14</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E5" s="3">
+        <v>584</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="K5" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="L5" s="3" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="3">
+        <v>1898</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="F6" s="7">
+        <v>16.498850999999998</v>
+      </c>
+      <c r="G6" s="6">
+        <v>7.4838120000000004</v>
+      </c>
+      <c r="H6" s="6">
+        <v>4.47</v>
+      </c>
+      <c r="I6" s="6">
+        <v>12.08</v>
+      </c>
+      <c r="J6" s="7">
+        <v>14.14</v>
+      </c>
+      <c r="K6" s="6">
+        <v>22.297499999999999</v>
+      </c>
+      <c r="L6" s="6">
+        <v>35.409999999999997</v>
+      </c>
+      <c r="M6" s="8">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="3">
+        <v>1898</v>
+      </c>
+      <c r="C7" s="3">
+        <v>2</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" s="3">
+        <v>1351</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="J7" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="K7" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="L7" s="3" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="3">
+        <v>1162</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>213</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>213</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>213</v>
+      </c>
+      <c r="F8" s="3">
+        <v>4.3442340000000002</v>
+      </c>
+      <c r="G8" s="3">
+        <v>0.74147799999999997</v>
+      </c>
+      <c r="H8" s="3">
+        <v>3</v>
+      </c>
+      <c r="I8" s="3">
+        <v>4</v>
+      </c>
+      <c r="J8" s="3">
+        <v>5</v>
+      </c>
+      <c r="K8" s="3">
+        <v>5</v>
+      </c>
+      <c r="L8" s="3">
+        <v>5</v>
+      </c>
+      <c r="M8" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="3">
+        <v>1898</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="F9" s="3">
+        <v>27.371970000000001</v>
+      </c>
+      <c r="G9" s="3">
+        <v>4.6324810000000003</v>
+      </c>
+      <c r="H9" s="3">
+        <v>20</v>
+      </c>
+      <c r="I9" s="3">
+        <v>23</v>
+      </c>
+      <c r="J9" s="3">
+        <v>27</v>
+      </c>
+      <c r="K9" s="3">
+        <v>31</v>
+      </c>
+      <c r="L9" s="3">
+        <v>35</v>
+      </c>
+      <c r="M9" s="2">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="3">
+        <v>1898</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="F10" s="7">
+        <v>24.161749</v>
+      </c>
+      <c r="G10" s="6">
+        <v>4.9726369999999998</v>
+      </c>
+      <c r="H10" s="6">
+        <v>15</v>
+      </c>
+      <c r="I10" s="6">
+        <v>20</v>
+      </c>
+      <c r="J10" s="7">
+        <v>25</v>
+      </c>
+      <c r="K10" s="6">
+        <v>28</v>
+      </c>
+      <c r="L10" s="6">
+        <v>33</v>
+      </c>
+      <c r="M10" s="8">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="H12" s="2">
+        <f>I10-H10</f>
+        <v>5</v>
+      </c>
+      <c r="I12" s="2">
+        <f>J10-I10</f>
+        <v>5</v>
+      </c>
+      <c r="K12" s="2">
+        <f>K10-J10</f>
+        <v>3</v>
+      </c>
+      <c r="L12" s="2">
+        <f>L10-K10</f>
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Finalize FoodHub project: added conclusions, recommendations, and cleaned workspace
</commit_message>
<xml_diff>
--- a/data/foodhub_order.xlsx
+++ b/data/foodhub_order.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/bf891bf09a799b20/DataAnalytics/Python/FoodHub/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="45" documentId="8_{64E6E1D9-BDB5-47F1-9F78-93007192BD7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1185E050-C3C4-4CAD-A18E-5BC98C2A3189}"/>
+  <xr:revisionPtr revIDLastSave="60" documentId="8_{64E6E1D9-BDB5-47F1-9F78-93007192BD7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{32989B2C-C320-4675-B8E7-57F86251FBCE}"/>
   <bookViews>
     <workbookView xWindow="-23136" yWindow="3216" windowWidth="23232" windowHeight="13872" xr2:uid="{5BAA1057-82F7-459F-B01D-6D1C5E63EE43}"/>
   </bookViews>
@@ -842,7 +842,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="36">
+  <fills count="37">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1040,6 +1040,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="11">
     <border>
@@ -1216,7 +1222,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="13" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1236,6 +1242,7 @@
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="13" fillId="36" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1292,6 +1299,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1611,10 +1622,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51B2ACA2-0467-45E3-B735-4A297B099BB0}">
-  <dimension ref="A1:I1899"/>
+  <dimension ref="A1:I1048575"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1636,16 +1648,16 @@
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="9" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="9" t="s">
         <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
@@ -56698,6 +56710,12 @@
       </c>
       <c r="I1899">
         <v>24</v>
+      </c>
+    </row>
+    <row r="1048575" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E1048575">
+        <f>SUM(E2:E1048574)</f>
+        <v>31314.820000000058</v>
       </c>
     </row>
   </sheetData>

</xml_diff>